<commit_message>
Tested minor modifications to kSVRG methods...
</commit_message>
<xml_diff>
--- a/probLS/Documentation/RunResults.xlsx
+++ b/probLS/Documentation/RunResults.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanya/Documents/GitWorkspaces/slbfgs/probLS/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C2CCA15-5FC5-4A4A-9E02-9B1F2601AED6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361C04AD-AD39-7B4E-AF4E-BAF44CBF87BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{08CD8C98-9756-DA47-A790-32C071640A96}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -497,7 +497,7 @@
   <dimension ref="A1:CV29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection sqref="A1:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Further updates and tests to the MATLAB kSVRG methods
</commit_message>
<xml_diff>
--- a/probLS/Documentation/RunResults.xlsx
+++ b/probLS/Documentation/RunResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanya/Documents/GitWorkspaces/slbfgs/probLS/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361C04AD-AD39-7B4E-AF4E-BAF44CBF87BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9E3387-B51B-8040-9E08-25EC7FA2839E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1780" windowWidth="28040" windowHeight="17440" xr2:uid="{08CD8C98-9756-DA47-A790-32C071640A96}"/>
+    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{08CD8C98-9756-DA47-A790-32C071640A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:CV29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H17"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>